<commit_message>
recalculate rates using pure decades
</commit_message>
<xml_diff>
--- a/Results/Plot data/ipcc_ar6_figure_sectors.xlsx
+++ b/Results/Plot data/ipcc_ar6_figure_sectors.xlsx
@@ -15,14 +15,16 @@
     <sheet name="Industry regions" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Transport trend" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Transport regions" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="AFOLU trend" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="AFOLU regions" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Buildings trend" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Buildings regions" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="AFOLU trend" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="AFOLU regions" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t xml:space="preserve">Author</t>
   </si>
@@ -33,7 +35,7 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-08-25</t>
+    <t xml:space="preserve">2021-09-13</t>
   </si>
   <si>
     <t xml:space="preserve">Units</t>
@@ -283,6 +285,45 @@
   </si>
   <si>
     <t xml:space="preserve">Intl. Shipping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-residential (direct CO2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential (direct CO2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All buildings (non-CO2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-residential (indirect CO2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential (indirect CO2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-residential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-CO2 (all buildings)</t>
   </si>
   <si>
     <t xml:space="preserve">Enteric Fermentation (CH4)</t>
@@ -788,689 +829,493 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>7.1</v>
+      <c r="A2" t="s">
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C2" t="n">
-        <v>2.45933548371225</v>
+        <v>0.782237072260382</v>
       </c>
       <c r="D2" t="n">
-        <v>2.46201671373278</v>
+        <v>0.791288297103925</v>
       </c>
       <c r="E2" t="n">
-        <v>2.46411423377595</v>
+        <v>0.717847259886038</v>
       </c>
       <c r="F2" t="n">
-        <v>2.45666946519945</v>
+        <v>0.716743247054865</v>
       </c>
       <c r="G2" t="n">
-        <v>2.47736723792027</v>
+        <v>0.715681571742592</v>
       </c>
       <c r="H2" t="n">
-        <v>2.48814763277207</v>
+        <v>0.735063463237398</v>
       </c>
       <c r="I2" t="n">
-        <v>2.49161801935487</v>
+        <v>0.785941597987959</v>
       </c>
       <c r="J2" t="n">
-        <v>2.44793516194359</v>
+        <v>0.760259484824698</v>
       </c>
       <c r="K2" t="n">
-        <v>2.45438592487034</v>
+        <v>0.727245010804661</v>
       </c>
       <c r="L2" t="n">
-        <v>2.46278713184064</v>
+        <v>0.757924518337373</v>
       </c>
       <c r="M2" t="n">
-        <v>2.4761574940428</v>
+        <v>0.713990436666469</v>
       </c>
       <c r="N2" t="n">
-        <v>2.4863035124547</v>
+        <v>0.72519979058931</v>
       </c>
       <c r="O2" t="n">
-        <v>2.5175102113773</v>
+        <v>0.733464669029646</v>
       </c>
       <c r="P2" t="n">
-        <v>2.5549201819782</v>
+        <v>0.768251138378626</v>
       </c>
       <c r="Q2" t="n">
-        <v>2.5947555171057</v>
+        <v>0.789134364869796</v>
       </c>
       <c r="R2" t="n">
-        <v>2.6176615791228</v>
+        <v>0.794265904040363</v>
       </c>
       <c r="S2" t="n">
-        <v>2.65135152162366</v>
+        <v>0.781794225036289</v>
       </c>
       <c r="T2" t="n">
-        <v>2.6883193419558</v>
+        <v>0.795548812403642</v>
       </c>
       <c r="U2" t="n">
-        <v>2.72102404502826</v>
+        <v>0.828886131796061</v>
       </c>
       <c r="V2" t="n">
-        <v>2.73474096881868</v>
+        <v>0.811056914058445</v>
       </c>
       <c r="W2" t="n">
-        <v>2.7460196593992</v>
+        <v>0.826898046685206</v>
       </c>
       <c r="X2" t="n">
-        <v>2.76494094739638</v>
+        <v>0.821676964808909</v>
       </c>
       <c r="Y2" t="n">
-        <v>2.79436270915476</v>
+        <v>0.812083321728632</v>
       </c>
       <c r="Z2" t="n">
-        <v>2.81140232820714</v>
+        <v>0.853123018326185</v>
       </c>
       <c r="AA2" t="n">
-        <v>2.8301127895944</v>
+        <v>0.832386322815831</v>
       </c>
       <c r="AB2" t="n">
-        <v>2.859896251773</v>
+        <v>0.846407807367462</v>
       </c>
       <c r="AC2" t="n">
-        <v>2.8934770531005</v>
+        <v>0.853747357739472</v>
       </c>
       <c r="AD2" t="n">
-        <v>2.9040858208971</v>
+        <v>0.854703764302396</v>
       </c>
       <c r="AE2" t="n">
-        <v>2.9263944815595</v>
+        <v>0.88398186197604</v>
       </c>
       <c r="AF2" t="n">
-        <v>2.96180337932477</v>
+        <v>0.902021999411506</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>7.2</v>
+      <c r="A3" t="s">
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C3" t="n">
-        <v>0.383572847364061</v>
+        <v>2.2214177847958</v>
       </c>
       <c r="D3" t="n">
-        <v>0.383795978256541</v>
+        <v>2.23311092948979</v>
       </c>
       <c r="E3" t="n">
-        <v>0.382274552513672</v>
+        <v>2.18722496654821</v>
       </c>
       <c r="F3" t="n">
-        <v>0.381423493556538</v>
+        <v>2.25224263015324</v>
       </c>
       <c r="G3" t="n">
-        <v>0.382807199299097</v>
+        <v>2.15937867851455</v>
       </c>
       <c r="H3" t="n">
-        <v>0.381443346461469</v>
+        <v>2.2217483095595</v>
       </c>
       <c r="I3" t="n">
-        <v>0.383036044598717</v>
+        <v>2.21723629954086</v>
       </c>
       <c r="J3" t="n">
-        <v>0.372349191527853</v>
+        <v>2.23291671698003</v>
       </c>
       <c r="K3" t="n">
-        <v>0.374996729636997</v>
+        <v>2.09445459736264</v>
       </c>
       <c r="L3" t="n">
-        <v>0.376200488838974</v>
+        <v>2.13469137212694</v>
       </c>
       <c r="M3" t="n">
-        <v>0.37839455306519</v>
+        <v>2.17041712371828</v>
       </c>
       <c r="N3" t="n">
-        <v>0.376447648456337</v>
+        <v>2.18277850025533</v>
       </c>
       <c r="O3" t="n">
-        <v>0.380598892652708</v>
+        <v>2.16884633998896</v>
       </c>
       <c r="P3" t="n">
-        <v>0.381796776019359</v>
+        <v>2.22283910041798</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.382775101836781</v>
+        <v>2.24707327534424</v>
       </c>
       <c r="R3" t="n">
-        <v>0.385890181320798</v>
+        <v>2.24593387471139</v>
       </c>
       <c r="S3" t="n">
-        <v>0.391060740945522</v>
+        <v>2.22168007438514</v>
       </c>
       <c r="T3" t="n">
-        <v>0.393256612273342</v>
+        <v>2.1987187791273</v>
       </c>
       <c r="U3" t="n">
-        <v>0.39800806482296</v>
+        <v>2.23023588782883</v>
       </c>
       <c r="V3" t="n">
-        <v>0.399311819799809</v>
+        <v>2.19738935809693</v>
       </c>
       <c r="W3" t="n">
-        <v>0.401395081907014</v>
+        <v>2.23353919159706</v>
       </c>
       <c r="X3" t="n">
-        <v>0.400351822699294</v>
+        <v>2.18867314947878</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.4041042781333</v>
+        <v>2.15069214820696</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.406102345072752</v>
+        <v>2.21385650534764</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.410387622401279</v>
+        <v>2.18474516126724</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.414285147492653</v>
+        <v>2.18752686556134</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.418637236772873</v>
+        <v>2.21324692550689</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.419093494198307</v>
+        <v>2.26828463679267</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.421405487301627</v>
+        <v>2.33194276933718</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.426016532913334</v>
+        <v>2.36981409146647</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>7.3</v>
+      <c r="A4" t="s">
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C4" t="n">
-        <v>1.05534627839291</v>
+        <v>0.0000096074973</v>
       </c>
       <c r="D4" t="n">
-        <v>1.0317234760671</v>
+        <v>0.00001733463429</v>
       </c>
       <c r="E4" t="n">
-        <v>1.0169913913399</v>
+        <v>0.000257126454216</v>
       </c>
       <c r="F4" t="n">
-        <v>0.984318566024592</v>
+        <v>0.00100253234333924</v>
       </c>
       <c r="G4" t="n">
-        <v>0.971551386029115</v>
+        <v>0.002754962056712</v>
       </c>
       <c r="H4" t="n">
-        <v>0.971990017640001</v>
+        <v>0.0131902843481268</v>
       </c>
       <c r="I4" t="n">
-        <v>0.965753042060205</v>
+        <v>0.0169212606606136</v>
       </c>
       <c r="J4" t="n">
-        <v>0.95656959353205</v>
+        <v>0.0194851446329564</v>
       </c>
       <c r="K4" t="n">
-        <v>0.932883571553136</v>
+        <v>0.0209475606067223</v>
       </c>
       <c r="L4" t="n">
-        <v>0.944176624768218</v>
+        <v>0.0219729970851676</v>
       </c>
       <c r="M4" t="n">
-        <v>0.904318794885239</v>
+        <v>0.0229579614540507</v>
       </c>
       <c r="N4" t="n">
-        <v>0.89236863319956</v>
+        <v>0.0229031730308853</v>
       </c>
       <c r="O4" t="n">
-        <v>0.883249559516007</v>
+        <v>0.0226595808748759</v>
       </c>
       <c r="P4" t="n">
-        <v>0.877548060477198</v>
+        <v>0.0226001385094726</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.908804233764674</v>
+        <v>0.0220026216104646</v>
       </c>
       <c r="R4" t="n">
-        <v>0.936237836431014</v>
+        <v>0.020978723754971</v>
       </c>
       <c r="S4" t="n">
-        <v>0.946401930483504</v>
+        <v>0.0219193984782238</v>
       </c>
       <c r="T4" t="n">
-        <v>0.952889777243406</v>
+        <v>0.0225266725741825</v>
       </c>
       <c r="U4" t="n">
-        <v>0.984307316427504</v>
+        <v>0.023433733475893</v>
       </c>
       <c r="V4" t="n">
-        <v>0.986278196022813</v>
+        <v>0.0248990328211924</v>
       </c>
       <c r="W4" t="n">
-        <v>1.00135607907052</v>
+        <v>0.026500634042933</v>
       </c>
       <c r="X4" t="n">
-        <v>1.00558602026034</v>
+        <v>0.027759364806421</v>
       </c>
       <c r="Y4" t="n">
-        <v>1.0062786496678</v>
+        <v>0.0282691065525918</v>
       </c>
       <c r="Z4" t="n">
-        <v>1.01792373138421</v>
+        <v>0.0292118475549576</v>
       </c>
       <c r="AA4" t="n">
-        <v>1.01056352240653</v>
+        <v>0.0304495110795046</v>
       </c>
       <c r="AB4" t="n">
-        <v>1.00571330714784</v>
+        <v>0.0311737390923678</v>
       </c>
       <c r="AC4" t="n">
-        <v>1.00693226861854</v>
+        <v>0.029384066109529</v>
       </c>
       <c r="AD4" t="n">
-        <v>1.02390288030953</v>
+        <v>0.0276579708324134</v>
       </c>
       <c r="AE4" t="n">
-        <v>1.02340424632149</v>
+        <v>0.0250081179255853</v>
       </c>
       <c r="AF4" t="n">
-        <v>1.01757779807094</v>
+        <v>0.0241768397175773</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>7.4</v>
+      <c r="A5" t="s">
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C5" t="n">
-        <v>0.22387794466674</v>
+        <v>1.33552857214105</v>
       </c>
       <c r="D5" t="n">
-        <v>0.21862511868288</v>
+        <v>1.37238002662277</v>
       </c>
       <c r="E5" t="n">
-        <v>0.21869077349301</v>
+        <v>1.42128111007372</v>
       </c>
       <c r="F5" t="n">
-        <v>0.22768894380687</v>
+        <v>1.41133696799567</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2275694438745</v>
+        <v>1.4637608199865</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2325122696169</v>
+        <v>1.50439346719327</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2436810485109</v>
+        <v>1.61139998148989</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2451393931077</v>
+        <v>1.71005471241262</v>
       </c>
       <c r="K5" t="n">
-        <v>0.25246362121071</v>
+        <v>1.787239581708</v>
       </c>
       <c r="L5" t="n">
-        <v>0.255654358596</v>
+        <v>1.82394269276242</v>
       </c>
       <c r="M5" t="n">
-        <v>0.24796696854384</v>
+        <v>1.89577844920498</v>
       </c>
       <c r="N5" t="n">
-        <v>0.25128023645361</v>
+        <v>1.96835168158698</v>
       </c>
       <c r="O5" t="n">
-        <v>0.2490003589164</v>
+        <v>1.98157791036679</v>
       </c>
       <c r="P5" t="n">
-        <v>0.2588086651059</v>
+        <v>2.06701653203789</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.2637648212745</v>
+        <v>2.14857484030859</v>
       </c>
       <c r="R5" t="n">
-        <v>0.261774636123</v>
+        <v>2.26358385214573</v>
       </c>
       <c r="S5" t="n">
-        <v>0.2706979556736</v>
+        <v>2.31148537614831</v>
       </c>
       <c r="T5" t="n">
-        <v>0.2833067614923</v>
+        <v>2.42099524086986</v>
       </c>
       <c r="U5" t="n">
-        <v>0.2745988270662</v>
+        <v>2.47385727420246</v>
       </c>
       <c r="V5" t="n">
-        <v>0.2885626689309</v>
+        <v>2.42452618907847</v>
       </c>
       <c r="W5" t="n">
-        <v>0.3019052139831</v>
+        <v>2.51311496912207</v>
       </c>
       <c r="X5" t="n">
-        <v>0.3130500940476</v>
+        <v>2.53658094518465</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.3140219220684</v>
+        <v>2.59176077044486</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.321182098419</v>
+        <v>2.62379308287586</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.3242053603152</v>
+        <v>2.60357587550001</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.3220732672248</v>
+        <v>2.61602262191674</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.3358001889606</v>
+        <v>2.61096764719657</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.3373580553252</v>
+        <v>2.60595292124352</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.333238861956</v>
+        <v>2.60588300465813</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.342983277350877</v>
+        <v>2.55319452622767</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>7.5</v>
+      <c r="A6" t="s">
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C6" t="n">
-        <v>1.05759672099974</v>
+        <v>2.03976254649409</v>
       </c>
       <c r="D6" t="n">
-        <v>1.05182669506748</v>
+        <v>2.08590741714726</v>
       </c>
       <c r="E6" t="n">
-        <v>1.05462055431666</v>
+        <v>2.15151761769233</v>
       </c>
       <c r="F6" t="n">
-        <v>1.05119770389105</v>
+        <v>2.27811572761288</v>
       </c>
       <c r="G6" t="n">
-        <v>1.06957913748096</v>
+        <v>2.29610399181622</v>
       </c>
       <c r="H6" t="n">
-        <v>1.07494830418154</v>
+        <v>2.34327507309277</v>
       </c>
       <c r="I6" t="n">
-        <v>1.09077145914147</v>
+        <v>2.46410931859771</v>
       </c>
       <c r="J6" t="n">
-        <v>1.09148234620398</v>
+        <v>2.53152039247594</v>
       </c>
       <c r="K6" t="n">
-        <v>1.10023964086236</v>
+        <v>2.62424114439801</v>
       </c>
       <c r="L6" t="n">
-        <v>1.1076592179547</v>
+        <v>2.6351906952226</v>
       </c>
       <c r="M6" t="n">
-        <v>1.11973438088416</v>
+        <v>2.71867394064863</v>
       </c>
       <c r="N6" t="n">
-        <v>1.12772079667203</v>
+        <v>2.80671678562294</v>
       </c>
       <c r="O6" t="n">
-        <v>1.14152970347074</v>
+        <v>2.88427006191944</v>
       </c>
       <c r="P6" t="n">
-        <v>1.16423510294197</v>
+        <v>3.03407454651315</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.19089214965904</v>
+        <v>3.10226378991758</v>
       </c>
       <c r="R6" t="n">
-        <v>1.19983625356709</v>
+        <v>3.16001516735052</v>
       </c>
       <c r="S6" t="n">
-        <v>1.21046073796533</v>
+        <v>3.22227350988157</v>
       </c>
       <c r="T6" t="n">
-        <v>1.22230642789707</v>
+        <v>3.33107849080745</v>
       </c>
       <c r="U6" t="n">
-        <v>1.23917325230343</v>
+        <v>3.35903153743747</v>
       </c>
       <c r="V6" t="n">
-        <v>1.24603384276971</v>
+        <v>3.37406557941839</v>
       </c>
       <c r="W6" t="n">
-        <v>1.25950072252362</v>
+        <v>3.53750987451516</v>
       </c>
       <c r="X6" t="n">
-        <v>1.27203812248322</v>
+        <v>3.60893319007889</v>
       </c>
       <c r="Y6" t="n">
-        <v>1.27907606531659</v>
+        <v>3.68619225231231</v>
       </c>
       <c r="Z6" t="n">
-        <v>1.30468678587779</v>
+        <v>3.77072156188172</v>
       </c>
       <c r="AA6" t="n">
-        <v>1.32399033560017</v>
+        <v>3.75331821804164</v>
       </c>
       <c r="AB6" t="n">
-        <v>1.33347055265741</v>
+        <v>3.77966862185851</v>
       </c>
       <c r="AC6" t="n">
-        <v>1.35484919774142</v>
+        <v>3.80572631788251</v>
       </c>
       <c r="AD6" t="n">
-        <v>1.36755075369472</v>
+        <v>3.8361543123428</v>
       </c>
       <c r="AE6" t="n">
-        <v>1.37145481339971</v>
+        <v>3.93675111717429</v>
       </c>
       <c r="AF6" t="n">
-        <v>1.38943225584839</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>7.6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.0417228438687474</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.041114960814861</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.0422159545744509</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.0421768815824454</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.0429194967329475</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.0423361848771269</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.0439747433698536</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.0447849483740586</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.044754935372078</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.0457383998609597</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.045896350662276</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.0472578757228503</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.046843320694486</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0.0485011524965952</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.0503229436645571</v>
-      </c>
-      <c r="R7" t="n">
-        <v>0.0514009025436985</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0.0519885181384046</v>
-      </c>
-      <c r="T7" t="n">
-        <v>0.0538704099096563</v>
-      </c>
-      <c r="U7" t="n">
-        <v>0.0574411052544212</v>
-      </c>
-      <c r="V7" t="n">
-        <v>0.0569613655157462</v>
-      </c>
-      <c r="W7" t="n">
-        <v>0.0586617183431252</v>
-      </c>
-      <c r="X7" t="n">
-        <v>0.0610759978972377</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>0.0612628715444118</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>0.0641309264034442</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>0.0646451667985026</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>0.0646317753368652</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>0.0655018051173702</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>0.0686310699028617</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>0.0678147635914429</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>0.0682785057617064</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4.979180807728</v>
-      </c>
-      <c r="D8" t="n">
-        <v>4.93705854162133</v>
-      </c>
-      <c r="E8" t="n">
-        <v>4.94476376996267</v>
-      </c>
-      <c r="F8" t="n">
-        <v>4.95038710129067</v>
-      </c>
-      <c r="G8" t="n">
-        <v>4.92721480013867</v>
-      </c>
-      <c r="H8" t="n">
-        <v>4.89187336204267</v>
-      </c>
-      <c r="I8" t="n">
-        <v>4.829820287952</v>
-      </c>
-      <c r="J8" t="n">
-        <v>6.55340794822933</v>
-      </c>
-      <c r="K8" t="n">
-        <v>4.56696826829867</v>
-      </c>
-      <c r="L8" t="n">
-        <v>4.508682009712</v>
-      </c>
-      <c r="M8" t="n">
-        <v>5.05170398532267</v>
-      </c>
-      <c r="N8" t="n">
-        <v>4.88591768026667</v>
-      </c>
-      <c r="O8" t="n">
-        <v>5.50042406870933</v>
-      </c>
-      <c r="P8" t="n">
-        <v>5.665169111376</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>5.54685124291733</v>
-      </c>
-      <c r="R8" t="n">
-        <v>5.194334723936</v>
-      </c>
-      <c r="S8" t="n">
-        <v>5.48132627112533</v>
-      </c>
-      <c r="T8" t="n">
-        <v>4.80616361454933</v>
-      </c>
-      <c r="U8" t="n">
-        <v>4.97515829509867</v>
-      </c>
-      <c r="V8" t="n">
-        <v>5.86615657340267</v>
-      </c>
-      <c r="W8" t="n">
-        <v>5.33731686335467</v>
-      </c>
-      <c r="X8" t="n">
-        <v>5.06208077041067</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>5.444890438976</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>5.62006774946133</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>6.04309861895467</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>6.2484473756</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>5.69877314173867</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>5.573991504624</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>5.69026309869867</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>6.6050388476</v>
+        <v>3.89033861626895</v>
       </c>
     </row>
   </sheetData>
@@ -1514,11 +1359,1993 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.00717448439438151</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.00795425047144376</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0117625478145997</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0203601791380599</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0660410689393</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.082913595683</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0668002728021</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.0596915452242871</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0759297036844</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0934017348282</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.1441304431683</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.186691075755208</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.12400701329801</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.02809819501803</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.05406953069447</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0532778613503191</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.21166324322855</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.169205957322505</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.20709737917595</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.192873434105382</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0128504290669</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.016002509731</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0188043165829292</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.0192555223139106</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0104346994514</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0182452548438</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0273805196485</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0283513803947743</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.25246576301314</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.26989040560789</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.257424119881157</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.281228725046447</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0050838076711</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.013608014661</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0165578580651</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.0241430309338817</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0165868595132</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0146705184996</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0228710588521</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.0361492451492367</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0939694572236208</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.116731951558499</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.146142148289114</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.193208670183264</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0643601734725</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0800322251777</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0732847909436</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.0672835870968726</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.569059520364178</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.375110109207988</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.434203665809025</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.553715141419159</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.22428740384146</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.211863388427417</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.173997061423552</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.225797083988495</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.613544015013916</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.566946176528285</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.57306911892167</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.461994667205459</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0783909438771091</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0914286522559573</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.0947165747035948</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.0920532975995943</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.046689958762332</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.094291997270879</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.130361562123292</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.134648386739712</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.374081881491127</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.426943398279592</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.375072913109109</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.373782772291065</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.0498023490913937</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0694475439167402</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.0633957279075429</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.078779380025179</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.107232081658165</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.137621681095225</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.169295628366556</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.188551104917671</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.00338903536262018</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.000942251235256</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.00076491999683399</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0000075154212</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.00009739406052</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.00064982374071</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.0015710400621686</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.0000020920761</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.00639958275713254</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.009077084609999</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.00792316712071736</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.013071949273778</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.015831474456968</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.0139177125378574</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.0237871992341186</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.0337108309366679</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.074564827203941</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.0849768127529948</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.0972934936311822</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.165312289539716</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.221351665315118</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.219996099750201</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.0546313398291355</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.166720036934629</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.355637540219692</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.582100755445438</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.18537517033809</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.0956156948684523</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.160244447648057</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.166276092887987</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.272824100686088</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.352088938345596</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.433886671097859</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.308153397972236</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.0237809119055852</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.0466754691186954</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.065619137390984</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.0762046469399846</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.0392234598739972</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.0755992822477034</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.140260602331707</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.188328670615411</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.613753734179456</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.852955902072383</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.856509785501233</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.618798105139089</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.0256716225473477</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.0569016367592032</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.11294024147237</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.165072559561679</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.015684274862225</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.0365793906080139</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.0873898542091819</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.126070926083253</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.0592561486666638</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.089102900529898</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.119291529791057</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.161760937046576</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.129897783627961</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.158437851609889</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.20314309143464</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.176544352095003</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.0850496030040264</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.29896448350641</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.731313828805348</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1.2592742304695</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.303127882444229</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.375787467881588</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.306065721553889</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.286611076372164</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.560061141143064</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.509943642597959</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.49969803916729</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.331076723297067</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.0460026462925081</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.0718877932912505</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.106821543737207</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.115042902438672</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.0828869335106333</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.155839116501749</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.283301652163481</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.312422019026784</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.676043216355398</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.874966989866626</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.940591419514317</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.658330880891479</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.0244527986619492</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.0619449335840228</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.117823680681354</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.217552287519145</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.0450021854739792</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.130547653663943</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.226895909943916</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.366544118756054</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>7.1</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.45933548371225</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2.46201671373278</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.46411423377595</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2.45666946519945</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2.47736723792027</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2.48814763277207</v>
+      </c>
+      <c r="I2" t="n">
+        <v>2.49161801935487</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2.44793516194359</v>
+      </c>
+      <c r="K2" t="n">
+        <v>2.45438592487034</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2.46278713184064</v>
+      </c>
+      <c r="M2" t="n">
+        <v>2.4761574940428</v>
+      </c>
+      <c r="N2" t="n">
+        <v>2.4863035124547</v>
+      </c>
+      <c r="O2" t="n">
+        <v>2.5175102113773</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2.5549201819782</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>2.5947555171057</v>
+      </c>
+      <c r="R2" t="n">
+        <v>2.6176615791228</v>
+      </c>
+      <c r="S2" t="n">
+        <v>2.65135152162366</v>
+      </c>
+      <c r="T2" t="n">
+        <v>2.6883193419558</v>
+      </c>
+      <c r="U2" t="n">
+        <v>2.72102404502826</v>
+      </c>
+      <c r="V2" t="n">
+        <v>2.73474096881868</v>
+      </c>
+      <c r="W2" t="n">
+        <v>2.7460196593992</v>
+      </c>
+      <c r="X2" t="n">
+        <v>2.76494094739638</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>2.79436270915476</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>2.81140232820714</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>2.8301127895944</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>2.859896251773</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>2.8934770531005</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>2.9040858208971</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>2.9263944815595</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>2.96180337932477</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.383572847364061</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.383795978256541</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.382274552513672</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.381423493556538</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.382807199299097</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.381443346461469</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.383036044598717</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.372349191527853</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.374996729636997</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.376200488838974</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.37839455306519</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.376447648456337</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.380598892652708</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.381796776019359</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.382775101836781</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.385890181320798</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.391060740945522</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.393256612273342</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.39800806482296</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.399311819799809</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.401395081907014</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.400351822699294</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0.4041042781333</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.406102345072752</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0.410387622401279</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.414285147492653</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0.418637236772873</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0.419093494198307</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0.421405487301627</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0.426016532913334</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.05534627839291</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.0317234760671</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.0169913913399</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.984318566024592</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.971551386029115</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.971990017640001</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.965753042060205</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.95656959353205</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.932883571553136</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.944176624768218</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.904318794885239</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.89236863319956</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.883249559516007</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.877548060477198</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.908804233764674</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.936237836431014</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.946401930483504</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.952889777243406</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.984307316427504</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.986278196022813</v>
+      </c>
+      <c r="W4" t="n">
+        <v>1.00135607907052</v>
+      </c>
+      <c r="X4" t="n">
+        <v>1.00558602026034</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>1.0062786496678</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>1.01792373138421</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>1.01056352240653</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>1.00571330714784</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>1.00693226861854</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>1.02390288030953</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>1.02340424632149</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>1.01757779807094</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.22387794466674</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.21862511868288</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.21869077349301</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.22768894380687</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.2275694438745</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.2325122696169</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.2436810485109</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.2451393931077</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.25246362121071</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.255654358596</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.24796696854384</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.25128023645361</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.2490003589164</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.2588086651059</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.2637648212745</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.261774636123</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.2706979556736</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.2833067614923</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.2745988270662</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.2885626689309</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.3019052139831</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.3130500940476</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0.3140219220684</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.321182098419</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0.3242053603152</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0.3220732672248</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.3358001889606</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0.3373580553252</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0.333238861956</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0.342983277350877</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.05759672099974</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.05182669506748</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.05462055431666</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.05119770389105</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.06957913748096</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.07494830418154</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.09077145914147</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.09148234620398</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1.10023964086236</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1.1076592179547</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1.11973438088416</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1.12772079667203</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1.14152970347074</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1.16423510294197</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1.19089214965904</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1.19983625356709</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1.21046073796533</v>
+      </c>
+      <c r="T6" t="n">
+        <v>1.22230642789707</v>
+      </c>
+      <c r="U6" t="n">
+        <v>1.23917325230343</v>
+      </c>
+      <c r="V6" t="n">
+        <v>1.24603384276971</v>
+      </c>
+      <c r="W6" t="n">
+        <v>1.25950072252362</v>
+      </c>
+      <c r="X6" t="n">
+        <v>1.27203812248322</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>1.27907606531659</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>1.30468678587779</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>1.32399033560017</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>1.33347055265741</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>1.35484919774142</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>1.36755075369472</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>1.37145481339971</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>1.38943225584839</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0417228438687474</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.041114960814861</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0422159545744509</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0421768815824454</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0429194967329475</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.0423361848771269</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.0439747433698536</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.0447849483740586</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.044754935372078</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.0457383998609597</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.045896350662276</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.0472578757228503</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.046843320694486</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.0485011524965952</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.0503229436645571</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.0514009025436985</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.0519885181384046</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.0538704099096563</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.0574411052544212</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.0569613655157462</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.0586617183431252</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.0610759978972377</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0.0612628715444118</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.0641309264034442</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0.0646451667985026</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0.0646317753368652</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0.0655018051173702</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.0686310699028617</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0.0678147635914429</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0.0682785057617064</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4.979180807728</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4.93705854162133</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4.94476376996267</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4.95038710129067</v>
+      </c>
+      <c r="G8" t="n">
+        <v>4.92721480013867</v>
+      </c>
+      <c r="H8" t="n">
+        <v>4.89187336204267</v>
+      </c>
+      <c r="I8" t="n">
+        <v>4.829820287952</v>
+      </c>
+      <c r="J8" t="n">
+        <v>6.55340794822933</v>
+      </c>
+      <c r="K8" t="n">
+        <v>4.56696826829867</v>
+      </c>
+      <c r="L8" t="n">
+        <v>4.508682009712</v>
+      </c>
+      <c r="M8" t="n">
+        <v>5.05170398532267</v>
+      </c>
+      <c r="N8" t="n">
+        <v>4.88591768026667</v>
+      </c>
+      <c r="O8" t="n">
+        <v>5.50042406870933</v>
+      </c>
+      <c r="P8" t="n">
+        <v>5.665169111376</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>5.54685124291733</v>
+      </c>
+      <c r="R8" t="n">
+        <v>5.194334723936</v>
+      </c>
+      <c r="S8" t="n">
+        <v>5.48132627112533</v>
+      </c>
+      <c r="T8" t="n">
+        <v>4.80616361454933</v>
+      </c>
+      <c r="U8" t="n">
+        <v>4.97515829509867</v>
+      </c>
+      <c r="V8" t="n">
+        <v>5.86615657340267</v>
+      </c>
+      <c r="W8" t="n">
+        <v>5.33731686335467</v>
+      </c>
+      <c r="X8" t="n">
+        <v>5.06208077041067</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>5.444890438976</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>5.62006774946133</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>6.04309861895467</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>6.2484473756</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>5.69877314173867</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>5.573991504624</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>5.69026309869867</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>6.6050388476</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>49</v>
@@ -1544,7 +3371,7 @@
         <v>7.1</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>50</v>
@@ -1570,7 +3397,7 @@
         <v>7.1</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
@@ -1596,7 +3423,7 @@
         <v>7.1</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
         <v>54</v>
@@ -1622,7 +3449,7 @@
         <v>7.1</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
         <v>55</v>
@@ -1648,7 +3475,7 @@
         <v>7.1</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
         <v>56</v>
@@ -1674,7 +3501,7 @@
         <v>7.1</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
         <v>58</v>
@@ -1700,7 +3527,7 @@
         <v>7.1</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
         <v>60</v>
@@ -1726,7 +3553,7 @@
         <v>7.1</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
         <v>62</v>
@@ -1752,7 +3579,7 @@
         <v>7.1</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
         <v>64</v>
@@ -1778,7 +3605,7 @@
         <v>7.2</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
         <v>49</v>
@@ -1804,7 +3631,7 @@
         <v>7.2</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
         <v>50</v>
@@ -1830,7 +3657,7 @@
         <v>7.2</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
         <v>52</v>
@@ -1856,7 +3683,7 @@
         <v>7.2</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
         <v>54</v>
@@ -1882,7 +3709,7 @@
         <v>7.2</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C16" t="s">
         <v>55</v>
@@ -1908,7 +3735,7 @@
         <v>7.2</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
         <v>56</v>
@@ -1934,7 +3761,7 @@
         <v>7.2</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C18" t="s">
         <v>58</v>
@@ -1960,7 +3787,7 @@
         <v>7.2</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
         <v>60</v>
@@ -1986,7 +3813,7 @@
         <v>7.2</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
         <v>62</v>
@@ -2012,7 +3839,7 @@
         <v>7.2</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
         <v>64</v>
@@ -2038,7 +3865,7 @@
         <v>7.3</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
         <v>49</v>
@@ -2064,7 +3891,7 @@
         <v>7.3</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
         <v>50</v>
@@ -2090,7 +3917,7 @@
         <v>7.3</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
         <v>52</v>
@@ -2116,7 +3943,7 @@
         <v>7.3</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
         <v>54</v>
@@ -2142,7 +3969,7 @@
         <v>7.3</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
         <v>55</v>
@@ -2168,7 +3995,7 @@
         <v>7.3</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
         <v>56</v>
@@ -2194,7 +4021,7 @@
         <v>7.3</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s">
         <v>58</v>
@@ -2220,7 +4047,7 @@
         <v>7.3</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
         <v>60</v>
@@ -2246,7 +4073,7 @@
         <v>7.3</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
         <v>62</v>
@@ -2272,7 +4099,7 @@
         <v>7.3</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
         <v>64</v>
@@ -2298,7 +4125,7 @@
         <v>7.4</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
         <v>49</v>
@@ -2324,7 +4151,7 @@
         <v>7.4</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
         <v>50</v>
@@ -2350,7 +4177,7 @@
         <v>7.4</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C34" t="s">
         <v>52</v>
@@ -2376,7 +4203,7 @@
         <v>7.4</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
         <v>54</v>
@@ -2402,7 +4229,7 @@
         <v>7.4</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
         <v>55</v>
@@ -2428,7 +4255,7 @@
         <v>7.4</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
         <v>56</v>
@@ -2454,7 +4281,7 @@
         <v>7.4</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
         <v>58</v>
@@ -2480,7 +4307,7 @@
         <v>7.4</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
         <v>60</v>
@@ -2506,7 +4333,7 @@
         <v>7.4</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C40" t="s">
         <v>62</v>
@@ -2532,7 +4359,7 @@
         <v>7.4</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
         <v>64</v>
@@ -2558,7 +4385,7 @@
         <v>7.5</v>
       </c>
       <c r="B42" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s">
         <v>49</v>
@@ -2584,7 +4411,7 @@
         <v>7.5</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C43" t="s">
         <v>50</v>
@@ -2610,7 +4437,7 @@
         <v>7.5</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
         <v>52</v>
@@ -2636,7 +4463,7 @@
         <v>7.5</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C45" t="s">
         <v>54</v>
@@ -2662,7 +4489,7 @@
         <v>7.5</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C46" t="s">
         <v>55</v>
@@ -2688,7 +4515,7 @@
         <v>7.5</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C47" t="s">
         <v>56</v>
@@ -2714,7 +4541,7 @@
         <v>7.5</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C48" t="s">
         <v>58</v>
@@ -2740,7 +4567,7 @@
         <v>7.5</v>
       </c>
       <c r="B49" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C49" t="s">
         <v>60</v>
@@ -2766,7 +4593,7 @@
         <v>7.5</v>
       </c>
       <c r="B50" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C50" t="s">
         <v>62</v>
@@ -2792,7 +4619,7 @@
         <v>7.5</v>
       </c>
       <c r="B51" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C51" t="s">
         <v>64</v>
@@ -2818,7 +4645,7 @@
         <v>7.6</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C52" t="s">
         <v>49</v>
@@ -2844,7 +4671,7 @@
         <v>7.6</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C53" t="s">
         <v>50</v>
@@ -2870,7 +4697,7 @@
         <v>7.6</v>
       </c>
       <c r="B54" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C54" t="s">
         <v>52</v>
@@ -2896,7 +4723,7 @@
         <v>7.6</v>
       </c>
       <c r="B55" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C55" t="s">
         <v>54</v>
@@ -2922,7 +4749,7 @@
         <v>7.6</v>
       </c>
       <c r="B56" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C56" t="s">
         <v>55</v>
@@ -2948,7 +4775,7 @@
         <v>7.6</v>
       </c>
       <c r="B57" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C57" t="s">
         <v>56</v>
@@ -2974,7 +4801,7 @@
         <v>7.6</v>
       </c>
       <c r="B58" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C58" t="s">
         <v>58</v>
@@ -3000,7 +4827,7 @@
         <v>7.6</v>
       </c>
       <c r="B59" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C59" t="s">
         <v>60</v>
@@ -3026,7 +4853,7 @@
         <v>7.6</v>
       </c>
       <c r="B60" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C60" t="s">
         <v>62</v>
@@ -3052,7 +4879,7 @@
         <v>7.6</v>
       </c>
       <c r="B61" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C61" t="s">
         <v>64</v>
@@ -3078,7 +4905,7 @@
         <v>7.7</v>
       </c>
       <c r="B62" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C62" t="s">
         <v>49</v>
@@ -3104,7 +4931,7 @@
         <v>7.7</v>
       </c>
       <c r="B63" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C63" t="s">
         <v>50</v>
@@ -3130,7 +4957,7 @@
         <v>7.7</v>
       </c>
       <c r="B64" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C64" t="s">
         <v>52</v>
@@ -3156,7 +4983,7 @@
         <v>7.7</v>
       </c>
       <c r="B65" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C65" t="s">
         <v>54</v>
@@ -3182,7 +5009,7 @@
         <v>7.7</v>
       </c>
       <c r="B66" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C66" t="s">
         <v>55</v>
@@ -3208,7 +5035,7 @@
         <v>7.7</v>
       </c>
       <c r="B67" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C67" t="s">
         <v>56</v>
@@ -3234,7 +5061,7 @@
         <v>7.7</v>
       </c>
       <c r="B68" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C68" t="s">
         <v>58</v>
@@ -3260,7 +5087,7 @@
         <v>7.7</v>
       </c>
       <c r="B69" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C69" t="s">
         <v>60</v>
@@ -3286,7 +5113,7 @@
         <v>7.7</v>
       </c>
       <c r="B70" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C70" t="s">
         <v>62</v>
@@ -3312,7 +5139,7 @@
         <v>7.7</v>
       </c>
       <c r="B71" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C71" t="s">
         <v>64</v>
@@ -8185,93 +10012,95 @@
         <v>77</v>
       </c>
       <c r="C7" t="n">
-        <v>3.41669001758699</v>
+        <v>3.41792219246121</v>
       </c>
       <c r="D7" t="n">
-        <v>3.45676897420825</v>
+        <v>3.45757607616662</v>
       </c>
       <c r="E7" t="n">
-        <v>3.46376191806886</v>
+        <v>3.46404686352742</v>
       </c>
       <c r="F7" t="n">
-        <v>3.40929715799476</v>
+        <v>3.40989462421133</v>
       </c>
       <c r="G7" t="n">
-        <v>3.38776190194227</v>
+        <v>3.38842794888812</v>
       </c>
       <c r="H7" t="n">
-        <v>3.44423011306117</v>
+        <v>3.44465325656433</v>
       </c>
       <c r="I7" t="n">
-        <v>3.5490040177329</v>
+        <v>3.54997776316347</v>
       </c>
       <c r="J7" t="n">
-        <v>3.5905025425201</v>
+        <v>3.59071346653267</v>
       </c>
       <c r="K7" t="n">
-        <v>3.59401337352277</v>
+        <v>3.59483638138928</v>
       </c>
       <c r="L7" t="n">
-        <v>3.6271261409945</v>
+        <v>3.62816531258544</v>
       </c>
       <c r="M7" t="n">
-        <v>3.86967360557024</v>
+        <v>3.87142624509067</v>
       </c>
       <c r="N7" t="n">
-        <v>3.89894702026822</v>
+        <v>3.90060125396769</v>
       </c>
       <c r="O7" t="n">
-        <v>3.89589033212267</v>
+        <v>3.89776293605283</v>
       </c>
       <c r="P7" t="n">
-        <v>4.17355271320558</v>
+        <v>4.17667050926456</v>
       </c>
       <c r="Q7" t="n">
-        <v>4.3721297116664</v>
+        <v>4.37480669892437</v>
       </c>
       <c r="R7" t="n">
-        <v>4.53543598229857</v>
+        <v>4.53606719676809</v>
       </c>
       <c r="S7" t="n">
-        <v>4.83379328059141</v>
+        <v>4.83288368326754</v>
       </c>
       <c r="T7" t="n">
-        <v>5.09825586069203</v>
+        <v>5.09771016011113</v>
       </c>
       <c r="U7" t="n">
-        <v>5.01657268109001</v>
+        <v>5.01702444555554</v>
       </c>
       <c r="V7" t="n">
-        <v>4.86900736200993</v>
+        <v>4.87148649049973</v>
       </c>
       <c r="W7" t="n">
-        <v>5.34541635611833</v>
+        <v>5.34738545899502</v>
       </c>
       <c r="X7" t="n">
-        <v>5.75037923859227</v>
+        <v>5.75055089176297</v>
       </c>
       <c r="Y7" t="n">
-        <v>5.8726591582406</v>
+        <v>5.87309593487977</v>
       </c>
       <c r="Z7" t="n">
-        <v>5.96795026533967</v>
+        <v>5.96925689083642</v>
       </c>
       <c r="AA7" t="n">
-        <v>5.93366173954319</v>
+        <v>6.00250317716586</v>
       </c>
       <c r="AB7" t="n">
-        <v>5.76586778311346</v>
+        <v>5.77902641896457</v>
       </c>
       <c r="AC7" t="n">
-        <v>5.7444144806862</v>
+        <v>5.76293808129366</v>
       </c>
       <c r="AD7" t="n">
-        <v>5.81830584576587</v>
+        <v>5.88611232154201</v>
       </c>
       <c r="AE7" t="n">
-        <v>5.97618454989376</v>
-      </c>
-      <c r="AF7"/>
+        <v>5.99250445331019</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>5.91220343950393</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9627,15 +11456,17 @@
         <v>49</v>
       </c>
       <c r="E52" t="n">
-        <v>0.113938363137148</v>
+        <v>0.113958891830143</v>
       </c>
       <c r="F52" t="n">
-        <v>0.136411174643877</v>
+        <v>0.135976301511597</v>
       </c>
       <c r="G52" t="n">
-        <v>0.193317234213058</v>
-      </c>
-      <c r="H52"/>
+        <v>0.192771240768272</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.197285290570162</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -9651,15 +11482,17 @@
         <v>51</v>
       </c>
       <c r="E53" t="n">
-        <v>0.272132279652648</v>
+        <v>0.271043503576372</v>
       </c>
       <c r="F53" t="n">
-        <v>0.259862586302268</v>
+        <v>0.259386917983712</v>
       </c>
       <c r="G53" t="n">
-        <v>0.261751567228312</v>
-      </c>
-      <c r="H53"/>
+        <v>0.261568708988904</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.238039986328131</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -9675,15 +11508,17 @@
         <v>53</v>
       </c>
       <c r="E54" t="n">
-        <v>0.514027416988254</v>
+        <v>0.514358541160338</v>
       </c>
       <c r="F54" t="n">
-        <v>1.02414491923078</v>
+        <v>1.02360539215416</v>
       </c>
       <c r="G54" t="n">
-        <v>2.49578295954892</v>
-      </c>
-      <c r="H54"/>
+        <v>2.50008537916415</v>
+      </c>
+      <c r="H54" t="n">
+        <v>3.2063601988074</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -9699,15 +11534,17 @@
         <v>54</v>
       </c>
       <c r="E55" t="n">
-        <v>0.682768661911839</v>
+        <v>0.684601916089539</v>
       </c>
       <c r="F55" t="n">
-        <v>0.405615331250279</v>
+        <v>0.406787753581197</v>
       </c>
       <c r="G55" t="n">
-        <v>0.394081554083868</v>
-      </c>
-      <c r="H55"/>
+        <v>0.395469498246991</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.347239741606149</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -9723,15 +11560,17 @@
         <v>55</v>
       </c>
       <c r="E56" t="n">
-        <v>0.903744247494496</v>
+        <v>0.903681814089596</v>
       </c>
       <c r="F56" t="n">
-        <v>0.647603384392035</v>
+        <v>0.647461398947509</v>
       </c>
       <c r="G56" t="n">
-        <v>0.592983851729057</v>
-      </c>
-      <c r="H56"/>
+        <v>0.591203083672208</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.435849101101599</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -9747,15 +11586,17 @@
         <v>57</v>
       </c>
       <c r="E57" t="n">
-        <v>0.0805973584994654</v>
+        <v>0.0807928046106435</v>
       </c>
       <c r="F57" t="n">
-        <v>0.136475302124244</v>
+        <v>0.136935108765845</v>
       </c>
       <c r="G57" t="n">
-        <v>0.179373135660304</v>
-      </c>
-      <c r="H57"/>
+        <v>0.180995142777548</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.174769645383652</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -9771,15 +11612,17 @@
         <v>59</v>
       </c>
       <c r="E58" t="n">
-        <v>0.038945367261123</v>
+        <v>0.0389489383551948</v>
       </c>
       <c r="F58" t="n">
-        <v>0.0760341498861561</v>
+        <v>0.0776824234748245</v>
       </c>
       <c r="G58" t="n">
-        <v>0.131295641535181</v>
-      </c>
-      <c r="H58"/>
+        <v>0.128429837587348</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.147940268791558</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -9795,15 +11638,17 @@
         <v>61</v>
       </c>
       <c r="E59" t="n">
-        <v>0.64504502769182</v>
+        <v>0.645086600550955</v>
       </c>
       <c r="F59" t="n">
-        <v>0.873715878175355</v>
+        <v>0.873624693777478</v>
       </c>
       <c r="G59" t="n">
-        <v>0.553906466109349</v>
-      </c>
-      <c r="H59"/>
+        <v>0.554238523420532</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.354218526374449</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -9819,15 +11664,17 @@
         <v>63</v>
       </c>
       <c r="E60" t="n">
-        <v>0.0469851911638804</v>
+        <v>0.0470993661974234</v>
       </c>
       <c r="F60" t="n">
-        <v>0.0967783877931061</v>
+        <v>0.0965519906916637</v>
       </c>
       <c r="G60" t="n">
-        <v>0.168190969859239</v>
-      </c>
-      <c r="H60"/>
+        <v>0.167840766503536</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.303732036928939</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -9843,15 +11690,17 @@
         <v>65</v>
       </c>
       <c r="E61" t="n">
-        <v>0.115878527237639</v>
+        <v>0.115887175986309</v>
       </c>
       <c r="F61" t="n">
-        <v>0.213012451934531</v>
+        <v>0.213721843959272</v>
       </c>
       <c r="G61" t="n">
-        <v>0.375378062514763</v>
-      </c>
-      <c r="H61"/>
+        <v>0.375741949213345</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.508529709310321</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10659,93 +12508,95 @@
         <v>77</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0886062798009365</v>
+        <v>0.0886853449007034</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0896939018311919</v>
+        <v>0.0897903217915766</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0882710614465292</v>
+        <v>0.0883725992530632</v>
       </c>
       <c r="F9" t="n">
-        <v>0.099056765295856</v>
+        <v>0.0991488651839166</v>
       </c>
       <c r="G9" t="n">
-        <v>0.105745091564769</v>
+        <v>0.105858329202258</v>
       </c>
       <c r="H9" t="n">
-        <v>0.103903760608469</v>
+        <v>0.10403451252605</v>
       </c>
       <c r="I9" t="n">
-        <v>0.114535127578119</v>
+        <v>0.114687751656906</v>
       </c>
       <c r="J9" t="n">
-        <v>0.109656158646305</v>
+        <v>0.109743060391944</v>
       </c>
       <c r="K9" t="n">
-        <v>0.106776794320295</v>
+        <v>0.106845995656227</v>
       </c>
       <c r="L9" t="n">
-        <v>0.108316463937004</v>
+        <v>0.108417029048586</v>
       </c>
       <c r="M9" t="n">
-        <v>0.115417906662685</v>
+        <v>0.11548557243016</v>
       </c>
       <c r="N9" t="n">
-        <v>0.11685519397752</v>
+        <v>0.116930219439312</v>
       </c>
       <c r="O9" t="n">
-        <v>0.124837043894704</v>
+        <v>0.124902769106974</v>
       </c>
       <c r="P9" t="n">
-        <v>0.137939814513159</v>
+        <v>0.1379554419719</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.14366383564934</v>
+        <v>0.143642395181647</v>
       </c>
       <c r="R9" t="n">
-        <v>0.144281721275816</v>
+        <v>0.144294496063851</v>
       </c>
       <c r="S9" t="n">
-        <v>0.151522518107678</v>
+        <v>0.151517498423984</v>
       </c>
       <c r="T9" t="n">
-        <v>0.156451637452382</v>
+        <v>0.156472827256572</v>
       </c>
       <c r="U9" t="n">
-        <v>0.156144555678002</v>
+        <v>0.1561546758553</v>
       </c>
       <c r="V9" t="n">
-        <v>0.156053215250889</v>
+        <v>0.156358345629016</v>
       </c>
       <c r="W9" t="n">
-        <v>0.167440588769771</v>
+        <v>0.167792136604479</v>
       </c>
       <c r="X9" t="n">
-        <v>0.182564717559806</v>
+        <v>0.182935144971207</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.187146647384374</v>
+        <v>0.187689989328915</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.19146530653241</v>
+        <v>0.192161923210904</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.186793074005122</v>
+        <v>0.186326717280975</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.189073333882637</v>
+        <v>0.189976872010531</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.191050180667319</v>
+        <v>0.192803908949096</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.204410618699142</v>
+        <v>0.204829114754359</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.211853742330227</v>
-      </c>
-      <c r="AF9"/>
+        <v>0.216505168803967</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>0.223253515355727</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12127,15 +13978,17 @@
         <v>49</v>
       </c>
       <c r="E53" t="n">
-        <v>0.004439663802929</v>
+        <v>0.00443995682455102</v>
       </c>
       <c r="F53" t="n">
-        <v>0.00414237279804412</v>
+        <v>0.00414300643617234</v>
       </c>
       <c r="G53" t="n">
-        <v>0.00422263233572844</v>
-      </c>
-      <c r="H53"/>
+        <v>0.00428454963748211</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.00476824503116521</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -12151,15 +14004,17 @@
         <v>51</v>
       </c>
       <c r="E54" t="n">
-        <v>0.0104781216717666</v>
+        <v>0.0104398452536671</v>
       </c>
       <c r="F54" t="n">
-        <v>0.0101327373134555</v>
+        <v>0.0101256453186241</v>
       </c>
       <c r="G54" t="n">
-        <v>0.010953198472917</v>
-      </c>
-      <c r="H54"/>
+        <v>0.0109547612847389</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.0119805986179793</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -12175,15 +14030,17 @@
         <v>53</v>
       </c>
       <c r="E55" t="n">
-        <v>0.00825134417291999</v>
+        <v>0.00825290785686212</v>
       </c>
       <c r="F55" t="n">
-        <v>0.0205273642725314</v>
+        <v>0.0205088233619523</v>
       </c>
       <c r="G55" t="n">
-        <v>0.061218468213415</v>
-      </c>
-      <c r="H55"/>
+        <v>0.0615472768395807</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.118879856828135</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -12199,15 +14056,17 @@
         <v>54</v>
       </c>
       <c r="E56" t="n">
-        <v>0.0238333000049506</v>
+        <v>0.0238358736896113</v>
       </c>
       <c r="F56" t="n">
-        <v>0.0321929971362796</v>
+        <v>0.0321886723766916</v>
       </c>
       <c r="G56" t="n">
-        <v>0.0403131298347068</v>
-      </c>
-      <c r="H56"/>
+        <v>0.0403245543171784</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.03874069539363</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -12223,15 +14082,17 @@
         <v>55</v>
       </c>
       <c r="E57" t="n">
-        <v>0.0295880488592229</v>
+        <v>0.0295966539067285</v>
       </c>
       <c r="F57" t="n">
-        <v>0.0314821531542541</v>
+        <v>0.0314799575487435</v>
       </c>
       <c r="G57" t="n">
-        <v>0.0267432423941939</v>
-      </c>
-      <c r="H57"/>
+        <v>0.0266977312009837</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.0197109255286363</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -12247,15 +14108,17 @@
         <v>57</v>
       </c>
       <c r="E58" t="n">
-        <v>0.00114377669840296</v>
+        <v>0.00114372086360974</v>
       </c>
       <c r="F58" t="n">
-        <v>0.00155882543438251</v>
+        <v>0.00155899971545634</v>
       </c>
       <c r="G58" t="n">
-        <v>0.00197235816552877</v>
-      </c>
-      <c r="H58"/>
+        <v>0.00196429669577553</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.00219924382053142</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -12271,15 +14134,17 @@
         <v>61</v>
       </c>
       <c r="E59" t="n">
-        <v>0.00361917150669259</v>
+        <v>0.00361941037511874</v>
       </c>
       <c r="F59" t="n">
-        <v>0.00430656110341844</v>
+        <v>0.00430611659222553</v>
       </c>
       <c r="G59" t="n">
-        <v>0.00470020157706697</v>
-      </c>
-      <c r="H59"/>
+        <v>0.00470301074814935</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.00680287365524965</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -12295,15 +14160,17 @@
         <v>63</v>
       </c>
       <c r="E60" t="n">
-        <v>0.000198302128773191</v>
+        <v>0.000297381190656857</v>
       </c>
       <c r="F60" t="n">
-        <v>0.000344552072386849</v>
+        <v>0.000405542183586099</v>
       </c>
       <c r="G60" t="n">
-        <v>0.00146132076288643</v>
-      </c>
-      <c r="H60"/>
+        <v>0.00145360514101307</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.00212950126643388</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -12319,15 +14186,17 @@
         <v>65</v>
       </c>
       <c r="E61" t="n">
-        <v>0.00421252752092204</v>
+        <v>0.00421280555135448</v>
       </c>
       <c r="F61" t="n">
-        <v>0.0102583928750111</v>
+        <v>0.0102873906861264</v>
       </c>
       <c r="G61" t="n">
-        <v>0.0145319999666626</v>
-      </c>
-      <c r="H61"/>
+        <v>0.014546708378107</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.0170438322866763</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adjusted biomass burning name
</commit_message>
<xml_diff>
--- a/Results/Plot data/ipcc_ar6_figure_sectors.xlsx
+++ b/Results/Plot data/ipcc_ar6_figure_sectors.xlsx
@@ -35,7 +35,7 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-09-28</t>
+    <t xml:space="preserve">2021-10-04</t>
   </si>
   <si>
     <t xml:space="preserve">Units</t>
@@ -341,7 +341,7 @@
     <t xml:space="preserve">Managed soils and pasture (CO2, N2O)</t>
   </si>
   <si>
-    <t xml:space="preserve">Biomass burning (CO2, CH4)</t>
+    <t xml:space="preserve">Biomass burning (CH4, N2O)</t>
   </si>
   <si>
     <t xml:space="preserve">LULUCF (CO2)</t>

</xml_diff>

<commit_message>
cmip comparison and general checking
</commit_message>
<xml_diff>
--- a/Results/Plot data/ipcc_ar6_figure_sectors.xlsx
+++ b/Results/Plot data/ipcc_ar6_figure_sectors.xlsx
@@ -5813,18 +5813,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI7"/>
+  <dimension ref="A1:AG7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI6" sqref="AI6"/>
+      <selection pane="bottomRight" activeCell="AG4" sqref="AG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>0.33811702522910347</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6126,7 +6126,7 @@
         <v>0.2388230920528078</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>0.21962081132537709</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>0.14753737330608074</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -6431,16 +6431,8 @@
         <f>AF6/$AF$7</f>
         <v>5.5901698086631015E-2</v>
       </c>
-      <c r="AH6">
-        <f>SUM(AF5:AF6,AF3)</f>
-        <v>26.133547575607381</v>
-      </c>
-      <c r="AI6">
-        <f>AH6/AF7</f>
-        <v>0.44226216344551955</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="AF7">
         <f>SUM(AF2:AF6)</f>
         <v>59.090624827612373</v>

</xml_diff>